<commit_message>
Cambio de imagen después de revisión de experto
Cambio de imagen después de revisión de experto  solicitudgrafica
CN_10_12
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado10/guion12/SolicitudGrafica_CN_10_12_CO.xlsx
+++ b/fuentes/contenidos/grado10/guion12/SolicitudGrafica_CN_10_12_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Desktop\Edición Planeta\CN_10_12_CO\CN_10_12_con correcc Vivi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LyzMarcela\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado10\guion12\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -611,29 +611,29 @@
     <t>Por favor realizar ilustración igual  la imagen guía</t>
   </si>
   <si>
-    <t xml:space="preserve">Códigos shutterstock  58870661 133287557
+    <t>Por favor realizar ilustración igual  la imagen guía. En días pasados me habías pasado esta propuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Códigos Shutterstock 209458648 -131075399 </t>
+  </si>
+  <si>
+    <t>Por favor realizar montaje igual a la imagen guía</t>
+  </si>
+  <si>
+    <t>Por favor realizar ilustración igual a la imagen guía</t>
+  </si>
+  <si>
+    <t>Código shutterstock 195046295</t>
+  </si>
+  <si>
+    <t>Fotografía</t>
+  </si>
+  <si>
+    <t>For favor realizar ilustración igual a la imagen guía.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Códigos shutterstock  58870661 44968867
 </t>
-  </si>
-  <si>
-    <t>Por favor realizar ilustración igual  la imagen guía. En días pasados me habías pasado esta propuesta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Códigos Shutterstock 209458648 -131075399 </t>
-  </si>
-  <si>
-    <t>Por favor realizar montaje igual a la imagen guía</t>
-  </si>
-  <si>
-    <t>Por favor realizar ilustración igual a la imagen guía</t>
-  </si>
-  <si>
-    <t>Código shutterstock 195046295</t>
-  </si>
-  <si>
-    <t>Fotografía</t>
-  </si>
-  <si>
-    <t>For favor realizar ilustración igual a la imagen guía.</t>
   </si>
 </sst>
 </file>
@@ -1846,49 +1846,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>1108363</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>60613</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>3853294</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1333500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
-        <xdr:cNvPicPr/>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:srcRect l="48201" t="35017" r="24134" b="44758"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="14815704" y="3792681"/>
-          <a:ext cx="2744931" cy="1272887"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
-            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
       <xdr:colOff>1099706</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>17317</xdr:rowOff>
@@ -1905,7 +1862,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1952,7 +1909,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:srcRect l="26307" t="15697" r="25492" b="19098"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -1995,7 +1952,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:srcRect l="45825" t="40753" r="19382" b="37814"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -2038,7 +1995,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2085,7 +2042,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2183,7 +2140,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2230,7 +2187,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:srcRect l="47013" t="47092" r="24983" b="31777"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -2238,6 +2195,92 @@
         <a:xfrm>
           <a:off x="14062364" y="14711796"/>
           <a:ext cx="3602181" cy="1117022"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>5195</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:srcRect l="26477" t="57960" r="43313" b="25136"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13707341" y="15906750"/>
+          <a:ext cx="1695450" cy="533400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{53640926-AAD7-44D8-BBD7-CCE9431645EC}">
+            <a14:shadowObscured xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>4095749</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1309687</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagen 12"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:srcRect l="26477" t="57960" r="43313" b="25136"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="14239874" y="3881438"/>
+          <a:ext cx="3571875" cy="1166812"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2972,9 +3015,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3307,7 +3350,7 @@
         <v>IMG02</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3380,7 +3423,7 @@
       </c>
       <c r="J12" s="64"/>
       <c r="K12" s="64" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
@@ -3393,7 +3436,7 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3423,7 +3466,7 @@
       </c>
       <c r="J13" s="64"/>
       <c r="K13" s="64" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -3466,7 +3509,7 @@
       </c>
       <c r="J14" s="64"/>
       <c r="K14" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
@@ -3509,7 +3552,7 @@
       </c>
       <c r="J15" s="66"/>
       <c r="K15" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
@@ -3552,7 +3595,7 @@
       </c>
       <c r="J16"/>
       <c r="K16" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -3565,14 +3608,14 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E17" s="63" t="s">
         <v>153</v>
@@ -3636,7 +3679,7 @@
       </c>
       <c r="J18" s="66"/>
       <c r="K18" s="66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>

</xml_diff>